<commit_message>
Test Extraction on Git ✨ 29 ธ.ค. 63 เวลา 16:55
</commit_message>
<xml_diff>
--- a/dataset/xlsx/timeline.xlsx
+++ b/dataset/xlsx/timeline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="372">
   <si>
     <t>Date</t>
   </si>
@@ -1127,6 +1127,9 @@
   </si>
   <si>
     <t>12/28/2020</t>
+  </si>
+  <si>
+    <t>12/29/2020</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1487,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I363"/>
+  <dimension ref="A1:I364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -12017,6 +12020,35 @@
         <v>60</v>
       </c>
     </row>
+    <row r="364" spans="1:9">
+      <c r="A364" t="s">
+        <v>371</v>
+      </c>
+      <c r="B364">
+        <v>155</v>
+      </c>
+      <c r="C364">
+        <v>4</v>
+      </c>
+      <c r="D364">
+        <v>150</v>
+      </c>
+      <c r="E364">
+        <v>1</v>
+      </c>
+      <c r="F364">
+        <v>6440</v>
+      </c>
+      <c r="G364">
+        <v>4184</v>
+      </c>
+      <c r="H364">
+        <v>2195</v>
+      </c>
+      <c r="I364">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New Spreading Wave Province
</commit_message>
<xml_diff>
--- a/dataset/xlsx/timeline.xlsx
+++ b/dataset/xlsx/timeline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="375">
   <si>
     <t>Date</t>
   </si>
@@ -1136,6 +1136,9 @@
   </si>
   <si>
     <t>12/31/2020</t>
+  </si>
+  <si>
+    <t>01/01/2021</t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I366"/>
+  <dimension ref="A1:I367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -12113,6 +12116,35 @@
         <v>61</v>
       </c>
     </row>
+    <row r="367" spans="1:9">
+      <c r="A367" t="s">
+        <v>374</v>
+      </c>
+      <c r="B367">
+        <v>279</v>
+      </c>
+      <c r="C367">
+        <v>33</v>
+      </c>
+      <c r="D367">
+        <v>244</v>
+      </c>
+      <c r="E367">
+        <v>2</v>
+      </c>
+      <c r="F367">
+        <v>7163</v>
+      </c>
+      <c r="G367">
+        <v>4273</v>
+      </c>
+      <c r="H367">
+        <v>2827</v>
+      </c>
+      <c r="I367">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test Extraction on Git ✨ 11 มี.ค. 64 เวลา 17:47
</commit_message>
<xml_diff>
--- a/dataset/xlsx/timeline.xlsx
+++ b/dataset/xlsx/timeline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="444">
   <si>
     <t>Date</t>
   </si>
@@ -1340,6 +1340,12 @@
   </si>
   <si>
     <t>03/09/2021</t>
+  </si>
+  <si>
+    <t>03/10/2021</t>
+  </si>
+  <si>
+    <t>03/11/2021</t>
   </si>
 </sst>
 </file>
@@ -1697,7 +1703,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I434"/>
+  <dimension ref="A1:I436"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -14289,6 +14295,64 @@
         <v>85</v>
       </c>
     </row>
+    <row r="435" spans="1:9">
+      <c r="A435" t="s">
+        <v>442</v>
+      </c>
+      <c r="B435">
+        <v>39</v>
+      </c>
+      <c r="C435">
+        <v>95</v>
+      </c>
+      <c r="D435">
+        <v>-56</v>
+      </c>
+      <c r="E435">
+        <v>0</v>
+      </c>
+      <c r="F435">
+        <v>26540</v>
+      </c>
+      <c r="G435">
+        <v>25946</v>
+      </c>
+      <c r="H435">
+        <v>509</v>
+      </c>
+      <c r="I435">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9">
+      <c r="A436" t="s">
+        <v>443</v>
+      </c>
+      <c r="B436">
+        <v>58</v>
+      </c>
+      <c r="C436">
+        <v>54</v>
+      </c>
+      <c r="D436">
+        <v>4</v>
+      </c>
+      <c r="E436">
+        <v>0</v>
+      </c>
+      <c r="F436">
+        <v>26598</v>
+      </c>
+      <c r="G436">
+        <v>26000</v>
+      </c>
+      <c r="H436">
+        <v>513</v>
+      </c>
+      <c r="I436">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test Extraction on Git ✨ 21 เม.ย. 64 เวลา 23:41
</commit_message>
<xml_diff>
--- a/dataset/xlsx/timeline.xlsx
+++ b/dataset/xlsx/timeline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="485">
   <si>
     <t>Date</t>
   </si>
@@ -1460,6 +1460,15 @@
   </si>
   <si>
     <t>04/18/2021</t>
+  </si>
+  <si>
+    <t>04/19/2021</t>
+  </si>
+  <si>
+    <t>04/20/2021</t>
+  </si>
+  <si>
+    <t>04/21/2021</t>
   </si>
 </sst>
 </file>
@@ -1817,7 +1826,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I474"/>
+  <dimension ref="A1:I477"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -15569,6 +15578,93 @@
         <v>101</v>
       </c>
     </row>
+    <row r="475" spans="1:9">
+      <c r="A475" t="s">
+        <v>482</v>
+      </c>
+      <c r="B475">
+        <v>1390</v>
+      </c>
+      <c r="C475">
+        <v>104</v>
+      </c>
+      <c r="D475">
+        <v>1283</v>
+      </c>
+      <c r="E475">
+        <v>3</v>
+      </c>
+      <c r="F475">
+        <v>43742</v>
+      </c>
+      <c r="G475">
+        <v>28787</v>
+      </c>
+      <c r="H475">
+        <v>14851</v>
+      </c>
+      <c r="I475">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="476" spans="1:9">
+      <c r="A476" t="s">
+        <v>483</v>
+      </c>
+      <c r="B476">
+        <v>1443</v>
+      </c>
+      <c r="C476">
+        <v>171</v>
+      </c>
+      <c r="D476">
+        <v>1268</v>
+      </c>
+      <c r="E476">
+        <v>4</v>
+      </c>
+      <c r="F476">
+        <v>45185</v>
+      </c>
+      <c r="G476">
+        <v>28958</v>
+      </c>
+      <c r="H476">
+        <v>16119</v>
+      </c>
+      <c r="I476">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="477" spans="1:9">
+      <c r="A477" t="s">
+        <v>484</v>
+      </c>
+      <c r="B477">
+        <v>1458</v>
+      </c>
+      <c r="C477">
+        <v>413</v>
+      </c>
+      <c r="D477">
+        <v>1043</v>
+      </c>
+      <c r="E477">
+        <v>2</v>
+      </c>
+      <c r="F477">
+        <v>46643</v>
+      </c>
+      <c r="G477">
+        <v>29371</v>
+      </c>
+      <c r="H477">
+        <v>17162</v>
+      </c>
+      <c r="I477">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test Extraction on Git ✨ 27 เม.ย. 64 เวลา 22:48
</commit_message>
<xml_diff>
--- a/dataset/xlsx/timeline.xlsx
+++ b/dataset/xlsx/timeline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="491">
   <si>
     <t>Date</t>
   </si>
@@ -1481,6 +1481,12 @@
   </si>
   <si>
     <t>04/25/2021</t>
+  </si>
+  <si>
+    <t>04/26/2021</t>
+  </si>
+  <si>
+    <t>04/27/2021</t>
   </si>
 </sst>
 </file>
@@ -1838,7 +1844,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I481"/>
+  <dimension ref="A1:I483"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -15793,6 +15799,64 @@
         <v>140</v>
       </c>
     </row>
+    <row r="482" spans="1:9">
+      <c r="A482" t="s">
+        <v>489</v>
+      </c>
+      <c r="B482">
+        <v>2048</v>
+      </c>
+      <c r="C482">
+        <v>480</v>
+      </c>
+      <c r="D482">
+        <v>1560</v>
+      </c>
+      <c r="E482">
+        <v>8</v>
+      </c>
+      <c r="F482">
+        <v>57508</v>
+      </c>
+      <c r="G482">
+        <v>31593</v>
+      </c>
+      <c r="H482">
+        <v>25767</v>
+      </c>
+      <c r="I482">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="483" spans="1:9">
+      <c r="A483" t="s">
+        <v>490</v>
+      </c>
+      <c r="B483">
+        <v>2179</v>
+      </c>
+      <c r="C483">
+        <v>1958</v>
+      </c>
+      <c r="D483">
+        <v>206</v>
+      </c>
+      <c r="E483">
+        <v>15</v>
+      </c>
+      <c r="F483">
+        <v>59687</v>
+      </c>
+      <c r="G483">
+        <v>33551</v>
+      </c>
+      <c r="H483">
+        <v>25973</v>
+      </c>
+      <c r="I483">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>